<commit_message>
.tex insertion function working
</commit_message>
<xml_diff>
--- a/Calculations/water_flow_table.xlsx
+++ b/Calculations/water_flow_table.xlsx
@@ -477,19 +477,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C2" t="n">
-        <v>2520.2685</v>
+        <v>2523.2685</v>
       </c>
       <c r="D2" t="n">
-        <v>-1680.179</v>
+        <v>-1682.179</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1680.179</v>
+        <v>1682.179</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -502,19 +502,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C3" t="n">
-        <v>2100.22375</v>
+        <v>2102.72375</v>
       </c>
       <c r="D3" t="n">
-        <v>-2100.22375</v>
+        <v>-2102.72375</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>2100.22375</v>
+        <v>2102.72375</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -527,19 +527,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C4" t="n">
-        <v>1680.179</v>
+        <v>1682.179</v>
       </c>
       <c r="D4" t="n">
-        <v>-2520.268499999999</v>
+        <v>-2523.268499999999</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>2520.268499999999</v>
+        <v>2523.268499999999</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -552,19 +552,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C5" t="n">
-        <v>1260.13425</v>
+        <v>1261.63425</v>
       </c>
       <c r="D5" t="n">
-        <v>-2940.313249999999</v>
+        <v>-2943.813249999999</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -577,19 +577,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C6" t="n">
-        <v>1260.13425</v>
+        <v>1261.63425</v>
       </c>
       <c r="D6" t="n">
-        <v>-2940.313249999999</v>
+        <v>-2943.813249999999</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -602,19 +602,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C7" t="n">
-        <v>1680.179</v>
+        <v>1682.179</v>
       </c>
       <c r="D7" t="n">
-        <v>-2520.268499999999</v>
+        <v>-2523.268499999999</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>2520.268499999999</v>
+        <v>2523.268499999999</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -627,19 +627,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C8" t="n">
-        <v>2520.2685</v>
+        <v>2523.2685</v>
       </c>
       <c r="D8" t="n">
-        <v>-1680.179</v>
+        <v>-1682.179</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1680.179</v>
+        <v>1682.179</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -652,19 +652,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C9" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="D9" t="n">
-        <v>-1260.13425</v>
+        <v>-1261.63425</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1260.13425</v>
+        <v>1261.63425</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -677,19 +677,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C10" t="n">
-        <v>3360.358</v>
+        <v>3364.358</v>
       </c>
       <c r="D10" t="n">
-        <v>-840.0894999999991</v>
+        <v>-841.0894999999991</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>840.0894999999991</v>
+        <v>841.0894999999991</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -702,19 +702,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C11" t="n">
-        <v>3780.40275</v>
+        <v>3784.90275</v>
       </c>
       <c r="D11" t="n">
-        <v>-420.0447499999996</v>
+        <v>-420.5447499999996</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>420.0447499999996</v>
+        <v>420.5447499999996</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C12" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -752,10 +752,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C13" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -777,22 +777,22 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C14" t="n">
-        <v>4620.49225</v>
+        <v>4625.99225</v>
       </c>
       <c r="D14" t="n">
-        <v>420.0447500000009</v>
+        <v>420.5447500000009</v>
       </c>
       <c r="E14" t="n">
-        <v>420.0447500000009</v>
+        <v>420.5447500000009</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>420.0447500000009</v>
+        <v>420.5447500000009</v>
       </c>
     </row>
     <row r="15">
@@ -802,22 +802,22 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C15" t="n">
-        <v>5040.536999999999</v>
+        <v>5046.536999999999</v>
       </c>
       <c r="D15" t="n">
-        <v>840.0895</v>
+        <v>841.0895</v>
       </c>
       <c r="E15" t="n">
-        <v>840.0895</v>
+        <v>841.0895</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>1260.134250000001</v>
+        <v>1261.634250000001</v>
       </c>
     </row>
     <row r="16">
@@ -827,22 +827,22 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C16" t="n">
-        <v>5460.58175</v>
+        <v>5467.08175</v>
       </c>
       <c r="D16" t="n">
-        <v>1260.134250000001</v>
+        <v>1261.634250000001</v>
       </c>
       <c r="E16" t="n">
-        <v>1260.134250000001</v>
+        <v>1261.634250000001</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>2520.268500000002</v>
+        <v>2523.268500000002</v>
       </c>
     </row>
     <row r="17">
@@ -852,22 +852,22 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C17" t="n">
-        <v>5880.626499999998</v>
+        <v>5887.626499999998</v>
       </c>
       <c r="D17" t="n">
-        <v>1680.178999999999</v>
+        <v>1682.178999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>1680.178999999999</v>
+        <v>1682.178999999999</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>4200.447500000001</v>
+        <v>4205.447500000001</v>
       </c>
     </row>
     <row r="18">
@@ -877,22 +877,22 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C18" t="n">
-        <v>6720.716</v>
+        <v>6728.716</v>
       </c>
       <c r="D18" t="n">
-        <v>2520.268500000001</v>
+        <v>2523.268500000001</v>
       </c>
       <c r="E18" t="n">
-        <v>2520.268500000001</v>
+        <v>2523.268500000001</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>6720.716000000002</v>
+        <v>6728.716000000002</v>
       </c>
     </row>
     <row r="19">
@@ -902,22 +902,22 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C19" t="n">
-        <v>7140.760749999999</v>
+        <v>7149.260749999999</v>
       </c>
       <c r="D19" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="E19" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>9661.029250000001</v>
+        <v>9672.529250000001</v>
       </c>
     </row>
     <row r="20">
@@ -927,22 +927,22 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C20" t="n">
-        <v>7980.850249999999</v>
+        <v>7990.350249999999</v>
       </c>
       <c r="D20" t="n">
-        <v>3780.402749999999</v>
+        <v>3784.902749999999</v>
       </c>
       <c r="E20" t="n">
-        <v>3780.402749999999</v>
+        <v>3784.902749999999</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>13441.432</v>
+        <v>13457.432</v>
       </c>
     </row>
     <row r="21">
@@ -952,22 +952,22 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C21" t="n">
-        <v>7560.805499999999</v>
+        <v>7569.805499999999</v>
       </c>
       <c r="D21" t="n">
-        <v>3360.358</v>
+        <v>3364.358</v>
       </c>
       <c r="E21" t="n">
-        <v>3360.358</v>
+        <v>3364.358</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>16801.79</v>
+        <v>16821.79</v>
       </c>
     </row>
     <row r="22">
@@ -977,22 +977,22 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C22" t="n">
-        <v>6720.716</v>
+        <v>6728.716</v>
       </c>
       <c r="D22" t="n">
-        <v>2520.268500000001</v>
+        <v>2523.268500000001</v>
       </c>
       <c r="E22" t="n">
-        <v>2520.268500000001</v>
+        <v>2523.268500000001</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>19322.0585</v>
+        <v>19345.0585</v>
       </c>
     </row>
     <row r="23">
@@ -1002,22 +1002,22 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C23" t="n">
-        <v>5040.536999999999</v>
+        <v>5046.536999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>840.0895</v>
+        <v>841.0895</v>
       </c>
       <c r="E23" t="n">
-        <v>840.0895</v>
+        <v>841.0895</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>20162.148</v>
+        <v>20186.148</v>
       </c>
     </row>
     <row r="24">
@@ -1027,22 +1027,22 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C24" t="n">
-        <v>3780.40275</v>
+        <v>3784.90275</v>
       </c>
       <c r="D24" t="n">
-        <v>-420.0447499999996</v>
+        <v>-420.5447499999996</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>420.0447499999996</v>
+        <v>420.5447499999996</v>
       </c>
       <c r="G24" t="n">
-        <v>19742.10325</v>
+        <v>19765.60325</v>
       </c>
     </row>
     <row r="25">
@@ -1052,22 +1052,22 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4200.447499999999</v>
+        <v>4205.447499999999</v>
       </c>
       <c r="C25" t="n">
-        <v>2940.313249999999</v>
+        <v>2943.813249999999</v>
       </c>
       <c r="D25" t="n">
-        <v>-1260.13425</v>
+        <v>-1261.63425</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>1260.13425</v>
+        <v>1261.63425</v>
       </c>
       <c r="G25" t="n">
-        <v>18481.969</v>
+        <v>18503.969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>